<commit_message>
add change req. (team member change )
</commit_message>
<xml_diff>
--- a/Requirements/change requests document.xlsx
+++ b/Requirements/change requests document.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Internet Banking System Main\Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internet-banking-system\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2964E9B-2021-42E4-B401-E99722C888BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3163298-C433-494C-8A5D-AE4E8778451B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Change Request ID</t>
   </si>
@@ -80,12 +79,28 @@
 6- change view client class
 7- tasks will be assigned on Trello.</t>
   </si>
+  <si>
+    <t>change_request_2</t>
+  </si>
+  <si>
+    <t>Team member change</t>
+  </si>
+  <si>
+    <t>1-Future tasks assignation (NON)
+2--Running tasks assignation (NON)
+3-Training needed
+4-Training for new member on her old team (NON)</t>
+  </si>
+  <si>
+    <t>1-Old team member and leader explained  plan, objective, documents, links and how we doing tasks for new member.
+-Expected time  (2 hrs).</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +111,14 @@
     <font>
       <b/>
       <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -128,13 +151,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,22 +475,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E32FEFA-CBE8-46B7-8B8E-BA71087C7CBE}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="39" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.140625" customWidth="1"/>
-    <col min="2" max="2" width="45.28515625" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="39" style="3"/>
+    <col min="3" max="3" width="46.85546875" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="39" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,7 +504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="255" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -490,6 +516,20 @@
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>